<commit_message>
Ini urang benerin lagi
Tadi si afif jadi dinosaurus, urg udah benerin
</commit_message>
<xml_diff>
--- a/Angkatan.xlsx
+++ b/Angkatan.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Documents\GitHub\koperasi_mawaddah\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20385" windowHeight="7950" activeTab="3"/>
+    <workbookView windowWidth="20385" windowHeight="8370" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -17,12 +12,12 @@
     <sheet name="NAMA ASC" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117">
   <si>
     <t>Aditya Dean Permana</t>
   </si>
@@ -378,8 +373,14 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -414,14 +415,151 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -434,8 +572,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -458,12 +782,251 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -477,16 +1040,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -507,34 +1073,74 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="10" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
+    <cellStyle name="Comma" xfId="2" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
+    <cellStyle name="Currency" xfId="5" builtinId="4"/>
+    <cellStyle name="Percent" xfId="6" builtinId="5"/>
+    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
+    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
+    <cellStyle name="Note" xfId="9" builtinId="10"/>
+    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
+    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
+    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Title" xfId="16" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
+    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
+    <cellStyle name="Input" xfId="21" builtinId="20"/>
+    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
+    <cellStyle name="Good" xfId="23" builtinId="26"/>
+    <cellStyle name="Output" xfId="24" builtinId="21"/>
+    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
+    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
+    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
+    <cellStyle name="Total" xfId="28" builtinId="25"/>
+    <cellStyle name="Bad" xfId="29" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
+    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
+    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
+    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
+    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
+    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
+    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
+    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -792,19 +1398,19 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:A98"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
   </cols>
@@ -815,12 +1421,12 @@
       </c>
     </row>
     <row r="2" spans="1:1">
-      <c r="A2" s="16" t="s">
+      <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1">
-      <c r="A3" s="16" t="s">
+      <c r="A3" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -840,7 +1446,7 @@
       </c>
     </row>
     <row r="7" spans="1:1">
-      <c r="A7" s="16" t="s">
+      <c r="A7" s="17" t="s">
         <v>6</v>
       </c>
     </row>
@@ -860,12 +1466,12 @@
       </c>
     </row>
     <row r="11" spans="1:1">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="17" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:1">
-      <c r="A12" s="16" t="s">
+      <c r="A12" s="17" t="s">
         <v>11</v>
       </c>
     </row>
@@ -875,7 +1481,7 @@
       </c>
     </row>
     <row r="14" spans="1:1">
-      <c r="A14" s="16" t="s">
+      <c r="A14" s="17" t="s">
         <v>13</v>
       </c>
     </row>
@@ -890,7 +1496,7 @@
       </c>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="16" t="s">
+      <c r="A17" s="17" t="s">
         <v>16</v>
       </c>
     </row>
@@ -915,17 +1521,17 @@
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="16" t="s">
+      <c r="A22" s="17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:1">
-      <c r="A23" s="16" t="s">
+      <c r="A23" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:1">
-      <c r="A24" s="16" t="s">
+      <c r="A24" s="17" t="s">
         <v>23</v>
       </c>
     </row>
@@ -945,7 +1551,7 @@
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="16" t="s">
+      <c r="A28" s="17" t="s">
         <v>27</v>
       </c>
     </row>
@@ -965,12 +1571,12 @@
       </c>
     </row>
     <row r="32" spans="1:1">
-      <c r="A32" s="16" t="s">
+      <c r="A32" s="17" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:1">
-      <c r="A33" s="16" t="s">
+      <c r="A33" s="17" t="s">
         <v>32</v>
       </c>
     </row>
@@ -985,7 +1591,7 @@
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="16" t="s">
+      <c r="A36" s="17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1025,12 +1631,12 @@
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="17" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:1">
-      <c r="A45" s="16" t="s">
+      <c r="A45" s="17" t="s">
         <v>44</v>
       </c>
     </row>
@@ -1040,7 +1646,7 @@
       </c>
     </row>
     <row r="47" spans="1:1">
-      <c r="A47" s="16" t="s">
+      <c r="A47" s="17" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1065,7 +1671,7 @@
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="16" t="s">
+      <c r="A52" s="17" t="s">
         <v>51</v>
       </c>
     </row>
@@ -1080,12 +1686,12 @@
       </c>
     </row>
     <row r="55" spans="1:1">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="17" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:1">
-      <c r="A56" s="16" t="s">
+      <c r="A56" s="17" t="s">
         <v>55</v>
       </c>
     </row>
@@ -1105,12 +1711,12 @@
       </c>
     </row>
     <row r="60" spans="1:1">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="17" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="61" spans="1:1">
-      <c r="A61" s="16" t="s">
+      <c r="A61" s="17" t="s">
         <v>60</v>
       </c>
     </row>
@@ -1120,17 +1726,17 @@
       </c>
     </row>
     <row r="63" spans="1:1">
-      <c r="A63" s="16" t="s">
+      <c r="A63" s="17" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:1">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="65" spans="1:1">
-      <c r="A65" s="16" t="s">
+      <c r="A65" s="17" t="s">
         <v>64</v>
       </c>
     </row>
@@ -1180,7 +1786,7 @@
       </c>
     </row>
     <row r="75" spans="1:1">
-      <c r="A75" s="16" t="s">
+      <c r="A75" s="17" t="s">
         <v>74</v>
       </c>
     </row>
@@ -1210,7 +1816,7 @@
       </c>
     </row>
     <row r="81" spans="1:1">
-      <c r="A81" s="16" t="s">
+      <c r="A81" s="17" t="s">
         <v>80</v>
       </c>
     </row>
@@ -1230,7 +1836,7 @@
       </c>
     </row>
     <row r="85" spans="1:1">
-      <c r="A85" s="16" t="s">
+      <c r="A85" s="17" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1245,7 +1851,7 @@
       </c>
     </row>
     <row r="88" spans="1:1">
-      <c r="A88" s="16" t="s">
+      <c r="A88" s="17" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1260,7 +1866,7 @@
       </c>
     </row>
     <row r="91" spans="1:1">
-      <c r="A91" s="16" t="s">
+      <c r="A91" s="17" t="s">
         <v>90</v>
       </c>
     </row>
@@ -1290,12 +1896,12 @@
       </c>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="16" t="s">
+      <c r="A97" s="17" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="98" spans="1:1">
-      <c r="A98" s="16" t="s">
+      <c r="A98" s="17" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1303,285 +1909,287 @@
   <sortState ref="A1:A98">
     <sortCondition ref="A1"/>
   </sortState>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="36" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="12.5714285714286" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="12" t="s">
+    <row r="1" ht="15.75" spans="1:2">
+      <c r="A1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="14" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="14" t="s">
+    <row r="2" ht="15.75" spans="1:2">
+      <c r="A2" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="16" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
-      <c r="A3" s="5" t="s">
+    <row r="3" ht="15.75" spans="1:2">
+      <c r="A3" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="3" t="s">
+      <c r="B3" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:2">
+      <c r="A4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="5" t="s">
+    <row r="5" ht="15.75" spans="1:2">
+      <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="3" t="s">
+    <row r="6" ht="15.75" spans="1:2">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="5" t="s">
+    <row r="7" ht="15.75" spans="1:2">
+      <c r="A7" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="3" t="s">
+    <row r="8" ht="15.75" spans="1:2">
+      <c r="A8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="5" t="s">
+    <row r="9" ht="15.75" spans="1:2">
+      <c r="A9" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
-      <c r="A10" s="3" t="s">
+    <row r="10" ht="15.75" spans="1:2">
+      <c r="A10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="5" t="s">
+    <row r="11" ht="15.75" spans="1:2">
+      <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+    <row r="12" ht="15.75" spans="1:2">
+      <c r="A12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="5" t="s">
+    <row r="13" ht="15.75" spans="1:2">
+      <c r="A13" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+    <row r="14" ht="15.75" spans="1:2">
+      <c r="A14" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="5" t="s">
+    <row r="15" ht="15.75" spans="1:2">
+      <c r="A15" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="3" t="s">
+    <row r="16" ht="15.75" spans="1:2">
+      <c r="A16" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
+      <c r="B16" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" ht="15.75" spans="1:2">
+      <c r="A17" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+    <row r="18" ht="15.75" spans="1:2">
+      <c r="A18" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
+    <row r="19" ht="15.75" spans="1:2">
+      <c r="A19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+    <row r="20" ht="15.75" spans="1:2">
+      <c r="A20" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
+    <row r="21" ht="15.75" spans="1:2">
+      <c r="A21" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="3" t="s">
+    <row r="22" ht="15.75" spans="1:2">
+      <c r="A22" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="5" t="s">
+    <row r="23" ht="15.75" spans="1:2">
+      <c r="A23" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="3" t="s">
+    <row r="24" ht="15.75" spans="1:2">
+      <c r="A24" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="5" t="s">
+    <row r="25" ht="15.75" spans="1:2">
+      <c r="A25" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
+    <row r="26" ht="15.75" spans="1:2">
+      <c r="A26" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="5" t="s">
+      <c r="B26" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" spans="1:2">
+      <c r="A27" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="3" t="s">
+    <row r="28" ht="15.75" spans="1:2">
+      <c r="A28" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="5" t="s">
+    <row r="29" ht="15.75" spans="1:2">
+      <c r="A29" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
+    <row r="30" ht="15.75" spans="1:2">
+      <c r="A30" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
-      <c r="A31" s="5" t="s">
+    <row r="31" ht="15.75" spans="1:2">
+      <c r="A31" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
-      <c r="A32" s="3" t="s">
+    <row r="32" ht="15.75" spans="1:2">
+      <c r="A32" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="5" t="s">
+    <row r="33" ht="15.75" spans="1:2">
+      <c r="A33" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -1594,7 +2202,7 @@
       </c>
     </row>
     <row r="35" spans="1:2">
-      <c r="A35" s="16" t="s">
+      <c r="A35" s="17" t="s">
         <v>5</v>
       </c>
       <c r="B35" t="s">
@@ -1658,7 +2266,7 @@
       </c>
     </row>
     <row r="43" spans="1:2">
-      <c r="A43" s="16" t="s">
+      <c r="A43" s="17" t="s">
         <v>34</v>
       </c>
       <c r="B43" t="s">
@@ -1666,7 +2274,7 @@
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="16" t="s">
+      <c r="A44" s="17" t="s">
         <v>38</v>
       </c>
       <c r="B44" t="s">
@@ -1682,7 +2290,7 @@
       </c>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="16" t="s">
+      <c r="A46" s="17" t="s">
         <v>41</v>
       </c>
       <c r="B46" t="s">
@@ -1722,7 +2330,7 @@
       </c>
     </row>
     <row r="51" spans="1:2">
-      <c r="A51" s="16" t="s">
+      <c r="A51" s="17" t="s">
         <v>58</v>
       </c>
       <c r="B51" t="s">
@@ -1746,7 +2354,7 @@
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="16" t="s">
+      <c r="A54" s="17" t="s">
         <v>67</v>
       </c>
       <c r="B54" t="s">
@@ -1754,7 +2362,7 @@
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="16" t="s">
+      <c r="A55" s="17" t="s">
         <v>68</v>
       </c>
       <c r="B55" t="s">
@@ -1786,7 +2394,7 @@
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="16" t="s">
+      <c r="A59" s="17" t="s">
         <v>81</v>
       </c>
       <c r="B59" t="s">
@@ -1794,14 +2402,14 @@
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="16" t="s">
+      <c r="A60" s="17" t="s">
         <v>85</v>
       </c>
       <c r="B60" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" ht="15.75" spans="1:2">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -1809,24 +2417,24 @@
         <v>105</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
-      <c r="A62" s="11" t="s">
+    <row r="62" ht="15.75" spans="1:2">
+      <c r="A62" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="9" t="s">
+    <row r="63" ht="15.75" spans="1:2">
+      <c r="A63" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="7" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="16" t="s">
+      <c r="A64" s="17" t="s">
         <v>1</v>
       </c>
       <c r="B64" t="s">
@@ -1906,7 +2514,7 @@
       </c>
     </row>
     <row r="74" spans="1:2">
-      <c r="A74" s="16" t="s">
+      <c r="A74" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B74" t="s">
@@ -1954,7 +2562,7 @@
       </c>
     </row>
     <row r="80" spans="1:2">
-      <c r="A80" s="16" t="s">
+      <c r="A80" s="17" t="s">
         <v>46</v>
       </c>
       <c r="B80" t="s">
@@ -1986,7 +2594,7 @@
       </c>
     </row>
     <row r="84" spans="1:2">
-      <c r="A84" s="16" t="s">
+      <c r="A84" s="17" t="s">
         <v>59</v>
       </c>
       <c r="B84" t="s">
@@ -2010,7 +2618,7 @@
       </c>
     </row>
     <row r="87" spans="1:2">
-      <c r="A87" s="16" t="s">
+      <c r="A87" s="17" t="s">
         <v>63</v>
       </c>
       <c r="B87" t="s">
@@ -2034,7 +2642,7 @@
       </c>
     </row>
     <row r="90" spans="1:2">
-      <c r="A90" s="16" t="s">
+      <c r="A90" s="17" t="s">
         <v>80</v>
       </c>
       <c r="B90" t="s">
@@ -2081,36 +2689,38 @@
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
-      <c r="A96" s="16"/>
+    <row r="96" spans="1:1">
+      <c r="A96" s="17"/>
     </row>
     <row r="97" spans="1:1">
-      <c r="A97" s="16"/>
+      <c r="A97" s="17"/>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:B97"/>
   <sheetViews>
     <sheetView topLeftCell="A67" workbookViewId="0">
       <selection activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7142857142857" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
-      <c r="A1" s="5" t="s">
+    <row r="1" ht="15.75" spans="1:2">
+      <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2146,7 +2756,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" ht="15.75" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -2154,27 +2764,27 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="3" t="s">
+    <row r="7" ht="15.75" spans="1:2">
+      <c r="A7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="5" t="s">
+    <row r="8" ht="15.75" spans="1:2">
+      <c r="A8" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="3" t="s">
+      <c r="B8" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" spans="1:2">
+      <c r="A9" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2226,7 +2836,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" ht="15.75" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>16</v>
       </c>
@@ -2234,35 +2844,35 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="5" t="s">
+    <row r="17" ht="15.75" spans="1:2">
+      <c r="A17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="B17" s="7" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="3" t="s">
+    <row r="18" ht="15.75" spans="1:2">
+      <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
-      <c r="A19" s="5" t="s">
+    <row r="19" ht="15.75" spans="1:2">
+      <c r="A19" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="3" t="s">
+    <row r="20" ht="15.75" spans="1:2">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B20" s="4" t="s">
+      <c r="B20" s="5" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2282,7 +2892,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" ht="15.75" spans="1:2">
       <c r="A23" s="1" t="s">
         <v>23</v>
       </c>
@@ -2290,19 +2900,19 @@
         <v>101</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
+    <row r="24" ht="15.75" spans="1:2">
+      <c r="A24" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="3" t="s">
+    <row r="25" ht="15.75" spans="1:2">
+      <c r="A25" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B25" s="4" t="s">
+      <c r="B25" s="5" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2314,7 +2924,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" ht="15.75" spans="1:2">
       <c r="A27" s="2" t="s">
         <v>27</v>
       </c>
@@ -2322,11 +2932,11 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="5" t="s">
+    <row r="28" ht="15.75" spans="1:2">
+      <c r="A28" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2378,7 +2988,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" ht="15.75" spans="1:2">
       <c r="A35" s="1" t="s">
         <v>35</v>
       </c>
@@ -2386,19 +2996,19 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="3" t="s">
+    <row r="36" ht="15.75" spans="1:2">
+      <c r="A36" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B36" s="4" t="s">
+      <c r="B36" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="5" t="s">
+    <row r="37" ht="15.75" spans="1:2">
+      <c r="A37" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2410,7 +3020,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" ht="15.75" spans="1:2">
       <c r="A39" s="1" t="s">
         <v>39</v>
       </c>
@@ -2418,15 +3028,15 @@
         <v>104</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="3" t="s">
+    <row r="40" ht="15.75" spans="1:2">
+      <c r="A40" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="4" t="s">
+      <c r="B40" s="5" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" ht="15.75" spans="1:2">
       <c r="A41" s="2" t="s">
         <v>41</v>
       </c>
@@ -2434,11 +3044,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="5" t="s">
+    <row r="42" ht="15.75" spans="1:2">
+      <c r="A42" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="7" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2466,7 +3076,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" ht="15.75" spans="1:2">
       <c r="A46" s="2" t="s">
         <v>46</v>
       </c>
@@ -2474,19 +3084,19 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
+    <row r="47" ht="15.75" spans="1:2">
+      <c r="A47" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="5" t="s">
+      <c r="B47" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" ht="15.75" spans="1:2">
+      <c r="A48" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2506,7 +3116,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" ht="15.75" spans="1:2">
       <c r="A51" s="1" t="s">
         <v>51</v>
       </c>
@@ -2514,19 +3124,19 @@
         <v>104</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="3" t="s">
+    <row r="52" ht="15.75" spans="1:2">
+      <c r="A52" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="5" t="s">
+    <row r="53" ht="15.75" spans="1:2">
+      <c r="A53" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="7" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2546,7 +3156,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" ht="15.75" spans="1:2">
       <c r="A56" s="1" t="s">
         <v>56</v>
       </c>
@@ -2554,11 +3164,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
-      <c r="A57" s="3" t="s">
+    <row r="57" ht="15.75" spans="1:2">
+      <c r="A57" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2578,7 +3188,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" ht="15.75" spans="1:2">
       <c r="A60" s="1" t="s">
         <v>60</v>
       </c>
@@ -2586,11 +3196,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="5" t="s">
+    <row r="61" ht="15.75" spans="1:2">
+      <c r="A61" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="7" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2666,7 +3276,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" ht="15.75" spans="1:2">
       <c r="A71" s="1" t="s">
         <v>71</v>
       </c>
@@ -2674,23 +3284,23 @@
         <v>98</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="3" t="s">
+    <row r="72" ht="15.75" spans="1:2">
+      <c r="A72" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="5" t="s">
+    <row r="73" ht="15.75" spans="1:2">
+      <c r="A73" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" ht="15.75" spans="1:2">
       <c r="A74" s="1" t="s">
         <v>74</v>
       </c>
@@ -2698,43 +3308,43 @@
         <v>105</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="3" t="s">
+    <row r="75" ht="15.75" spans="1:2">
+      <c r="A75" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B75" s="6" t="s">
+      <c r="B75" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
-      <c r="A76" s="5" t="s">
+    <row r="76" ht="15.75" spans="1:2">
+      <c r="A76" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B76" s="6" t="s">
+      <c r="B76" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="3" t="s">
+    <row r="77" ht="15.75" spans="1:2">
+      <c r="A77" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="5" t="s">
+      <c r="B77" s="7" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" ht="15.75" spans="1:2">
+      <c r="A78" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
-      <c r="A79" s="3" t="s">
+    <row r="79" ht="15.75" spans="1:2">
+      <c r="A79" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="6" t="s">
+      <c r="B79" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -2746,7 +3356,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" ht="15.75" spans="1:2">
       <c r="A81" s="2" t="s">
         <v>81</v>
       </c>
@@ -2754,11 +3364,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
-      <c r="A82" s="5" t="s">
+    <row r="82" ht="15.75" spans="1:2">
+      <c r="A82" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B82" s="6" t="s">
+      <c r="B82" s="7" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2786,7 +3396,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" ht="15.75" spans="1:2">
       <c r="A86" s="1" t="s">
         <v>87</v>
       </c>
@@ -2794,15 +3404,15 @@
         <v>98</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
-      <c r="A87" s="3" t="s">
+    <row r="87" ht="15.75" spans="1:2">
+      <c r="A87" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B87" s="6" t="s">
+      <c r="B87" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" ht="15.75" spans="1:2">
       <c r="A88" s="1" t="s">
         <v>90</v>
       </c>
@@ -2810,43 +3420,43 @@
         <v>102</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
-      <c r="A89" s="11" t="s">
+    <row r="89" ht="15.75" spans="1:2">
+      <c r="A89" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B89" s="6" t="s">
+      <c r="B89" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
-      <c r="A90" s="5" t="s">
+    <row r="90" ht="15.75" spans="1:2">
+      <c r="A90" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B90" s="6" t="s">
+      <c r="B90" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
-      <c r="A91" s="3" t="s">
+    <row r="91" ht="15.75" spans="1:2">
+      <c r="A91" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B91" s="6" t="s">
+      <c r="B91" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
-      <c r="A92" s="5" t="s">
+    <row r="92" ht="15.75" spans="1:2">
+      <c r="A92" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B92" s="6" t="s">
+      <c r="B92" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
-      <c r="A93" s="9" t="s">
+    <row r="93" ht="15.75" spans="1:2">
+      <c r="A93" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B93" s="6" t="s">
+      <c r="B93" s="7" t="s">
         <v>104</v>
       </c>
     </row>
@@ -2866,7 +3476,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:1">
       <c r="A96" s="2"/>
     </row>
     <row r="97" spans="1:1">
@@ -2876,58 +3486,60 @@
   <sortState ref="A2:B97">
     <sortCondition ref="A2"/>
   </sortState>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
   <dimension ref="A1:L97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="36" style="1" customWidth="1"/>
-    <col min="2" max="2" width="12.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.5714285714286" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.7142857142857" customWidth="1"/>
+    <col min="6" max="6" width="12.7142857142857" customWidth="1"/>
+    <col min="7" max="7" width="12.1428571428571" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" ht="15.75" spans="1:10">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-    </row>
-    <row r="2" spans="1:12">
-      <c r="A2" s="3" t="s">
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>99</v>
       </c>
       <c r="D2" t="str">
         <f>B1</f>
         <v>Agama</v>
       </c>
-      <c r="E2" t="str">
-        <f>B12</f>
-        <v>Dinosaurus</v>
+      <c r="E2" t="s">
+        <v>104</v>
       </c>
       <c r="F2" t="str">
         <f>B24</f>
@@ -2953,11 +3565,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
-      <c r="A3" s="5" t="s">
+    <row r="3" ht="15.75" spans="1:12">
+      <c r="A3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="7" t="s">
         <v>99</v>
       </c>
       <c r="D3">
@@ -2966,7 +3578,7 @@
       </c>
       <c r="E3">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="F3">
         <f t="shared" si="0"/>
@@ -2993,53 +3605,53 @@
       </c>
       <c r="L3">
         <f>SUM(D3:K3)</f>
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" spans="1:12">
       <c r="A4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="E4" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="8" t="s">
         <v>109</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="8" t="s">
         <v>110</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="H4" s="8" t="s">
         <v>111</v>
       </c>
-      <c r="I4" s="7" t="s">
+      <c r="I4" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="8" t="s">
         <v>113</v>
       </c>
-      <c r="K4" s="10" t="s">
+      <c r="K4" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="L4" s="11" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="5" spans="1:12">
-      <c r="A5" s="3" t="s">
+    <row r="5" ht="15.75" spans="1:2">
+      <c r="A5" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
         <v>44</v>
       </c>
@@ -3047,7 +3659,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
         <v>66</v>
       </c>
@@ -3055,7 +3667,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:2">
       <c r="A8" s="2" t="s">
         <v>67</v>
       </c>
@@ -3063,7 +3675,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:2">
       <c r="A9" s="1" t="s">
         <v>70</v>
       </c>
@@ -3071,7 +3683,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:2">
       <c r="A10" s="2" t="s">
         <v>80</v>
       </c>
@@ -3079,7 +3691,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:2">
       <c r="A11" s="1" t="s">
         <v>97</v>
       </c>
@@ -3087,7 +3699,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:2">
       <c r="A12" s="2" t="s">
         <v>1</v>
       </c>
@@ -3095,7 +3707,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
         <v>2</v>
       </c>
@@ -3103,7 +3715,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
@@ -3111,7 +3723,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:2">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
@@ -3119,7 +3731,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" ht="15.75" spans="1:2">
       <c r="A16" s="1" t="s">
         <v>39</v>
       </c>
@@ -3127,11 +3739,11 @@
         <v>104</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="3" t="s">
+    <row r="17" ht="15.75" spans="1:2">
+      <c r="A17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B17" s="5" t="s">
         <v>104</v>
       </c>
     </row>
@@ -3143,7 +3755,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" ht="15.75" spans="1:2">
       <c r="A19" s="2" t="s">
         <v>59</v>
       </c>
@@ -3151,47 +3763,47 @@
         <v>104</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="5" t="s">
+    <row r="20" ht="15.75" spans="1:2">
+      <c r="A20" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
-      <c r="A21" s="5" t="s">
+    <row r="21" ht="15.75" spans="1:2">
+      <c r="A21" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="5" t="s">
+    <row r="22" ht="15.75" spans="1:2">
+      <c r="A22" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="A23" s="9" t="s">
+    <row r="23" ht="15.75" spans="1:2">
+      <c r="A23" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="7" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
-      <c r="A24" s="5" t="s">
+    <row r="24" ht="15.75" spans="1:2">
+      <c r="A24" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" ht="15.75" spans="1:2">
       <c r="A25" s="1" t="s">
         <v>6</v>
       </c>
@@ -3199,43 +3811,43 @@
         <v>98</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
-      <c r="A26" s="3" t="s">
+    <row r="26" ht="15.75" spans="1:2">
+      <c r="A26" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B26" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
-      <c r="A27" s="5" t="s">
+    <row r="27" ht="15.75" spans="1:2">
+      <c r="A27" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="5" t="s">
+    <row r="28" ht="15.75" spans="1:2">
+      <c r="A28" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
-      <c r="A29" s="5" t="s">
+    <row r="29" ht="15.75" spans="1:2">
+      <c r="A29" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="7" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
-      <c r="A30" s="3" t="s">
+    <row r="30" ht="15.75" spans="1:2">
+      <c r="A30" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="B30" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3247,7 +3859,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" ht="15.75" spans="1:2">
       <c r="A32" s="1" t="s">
         <v>71</v>
       </c>
@@ -3255,11 +3867,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
-      <c r="A33" s="3" t="s">
+    <row r="33" ht="15.75" spans="1:2">
+      <c r="A33" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="7" t="s">
         <v>98</v>
       </c>
     </row>
@@ -3279,7 +3891,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" ht="15.75" spans="1:2">
       <c r="A36" s="1" t="s">
         <v>96</v>
       </c>
@@ -3287,11 +3899,11 @@
         <v>98</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="5" t="s">
+    <row r="37" ht="15.75" spans="1:2">
+      <c r="A37" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="7" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3359,7 +3971,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" ht="15.75" spans="1:2">
       <c r="A46" s="1" t="s">
         <v>45</v>
       </c>
@@ -3367,11 +3979,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
-      <c r="A47" s="3" t="s">
+    <row r="47" ht="15.75" spans="1:2">
+      <c r="A47" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="7" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3383,7 +3995,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" ht="15.75" spans="1:2">
       <c r="A49" s="2" t="s">
         <v>58</v>
       </c>
@@ -3391,11 +4003,11 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="3" t="s">
+    <row r="50" ht="15.75" spans="1:2">
+      <c r="A50" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="7" t="s">
         <v>100</v>
       </c>
     </row>
@@ -3407,7 +4019,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" ht="15.75" spans="1:2">
       <c r="A52" s="1" t="s">
         <v>12</v>
       </c>
@@ -3415,11 +4027,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
-      <c r="A53" s="3" t="s">
+    <row r="53" ht="15.75" spans="1:2">
+      <c r="A53" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B53" s="5" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3431,7 +4043,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" ht="15.75" spans="1:2">
       <c r="A55" s="1" t="s">
         <v>29</v>
       </c>
@@ -3439,11 +4051,11 @@
         <v>103</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
-      <c r="A56" s="3" t="s">
+    <row r="56" ht="15.75" spans="1:2">
+      <c r="A56" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="7" t="s">
         <v>103</v>
       </c>
     </row>
@@ -3455,7 +4067,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" ht="15.75" spans="1:2">
       <c r="A58" s="1" t="s">
         <v>65</v>
       </c>
@@ -3463,31 +4075,31 @@
         <v>103</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
-      <c r="A59" s="5" t="s">
+    <row r="59" ht="15.75" spans="1:2">
+      <c r="A59" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
-      <c r="A60" s="5" t="s">
+    <row r="60" ht="15.75" spans="1:2">
+      <c r="A60" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
-      <c r="A61" s="3" t="s">
+    <row r="61" ht="15.75" spans="1:2">
+      <c r="A61" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" ht="15.75" spans="1:2">
       <c r="A62" s="2" t="s">
         <v>85</v>
       </c>
@@ -3495,27 +4107,27 @@
         <v>103</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
-      <c r="A63" s="3" t="s">
+    <row r="63" ht="15.75" spans="1:2">
+      <c r="A63" s="4" t="s">
         <v>93</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
-      <c r="A64" s="5" t="s">
+    <row r="64" ht="15.75" spans="1:2">
+      <c r="A64" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="7" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
-      <c r="A65" s="3" t="s">
+    <row r="65" ht="15.75" spans="1:2">
+      <c r="A65" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B65" s="4" t="s">
+      <c r="B65" s="5" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3527,7 +4139,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" ht="15.75" spans="1:2">
       <c r="A67" s="1" t="s">
         <v>31</v>
       </c>
@@ -3535,11 +4147,11 @@
         <v>101</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
-      <c r="A68" s="5" t="s">
+    <row r="68" ht="15.75" spans="1:2">
+      <c r="A68" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="7" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3559,7 +4171,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" ht="15.75" spans="1:2">
       <c r="A71" s="1" t="s">
         <v>69</v>
       </c>
@@ -3567,39 +4179,39 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
-      <c r="A72" s="3" t="s">
+    <row r="72" ht="15.75" spans="1:2">
+      <c r="A72" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
-      <c r="A73" s="11" t="s">
+    <row r="73" ht="15.75" spans="1:2">
+      <c r="A73" s="12" t="s">
         <v>91</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="7" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
-      <c r="A74" s="5" t="s">
+    <row r="74" ht="15.75" spans="1:2">
+      <c r="A74" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
-      <c r="A75" s="3" t="s">
+    <row r="75" ht="15.75" spans="1:2">
+      <c r="A75" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B75" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" ht="15.75" spans="1:2">
       <c r="A76" s="1" t="s">
         <v>21</v>
       </c>
@@ -3607,19 +4219,19 @@
         <v>102</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
-      <c r="A77" s="5" t="s">
+    <row r="77" ht="15.75" spans="1:2">
+      <c r="A77" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B77" s="6" t="s">
+      <c r="B77" s="7" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
-      <c r="A78" s="5" t="s">
+    <row r="78" ht="15.75" spans="1:2">
+      <c r="A78" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B78" s="6" t="s">
+      <c r="B78" s="7" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3647,7 +4259,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" ht="15.75" spans="1:2">
       <c r="A82" s="1" t="s">
         <v>64</v>
       </c>
@@ -3655,11 +4267,11 @@
         <v>102</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
-      <c r="A83" s="3" t="s">
+    <row r="83" ht="15.75" spans="1:2">
+      <c r="A83" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B83" s="6" t="s">
+      <c r="B83" s="7" t="s">
         <v>102</v>
       </c>
     </row>
@@ -3743,7 +4355,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" ht="15.75" spans="1:2">
       <c r="A94" s="1" t="s">
         <v>86</v>
       </c>
@@ -3751,15 +4363,15 @@
         <v>105</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
-      <c r="A95" s="5" t="s">
+    <row r="95" ht="15.75" spans="1:2">
+      <c r="A95" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B95" s="6" t="s">
+      <c r="B95" s="7" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:1">
       <c r="A96" s="2"/>
     </row>
     <row r="97" spans="1:1">
@@ -3773,6 +4385,7 @@
   <mergeCells count="1">
     <mergeCell ref="D1:J1"/>
   </mergeCells>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>